<commit_message>
code update dntt khvu
</commit_message>
<xml_diff>
--- a/viettel_ns/Areas/QLVonDauTu/ReportExcelForm/KeHoachVonNam/rpt_BaoCao_KHNam_DonVi_Moi.xlsx
+++ b/viettel_ns/Areas/QLVonDauTu/ReportExcelForm/KeHoachVonNam/rpt_BaoCao_KHNam_DonVi_Moi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Minhvv\Code_Vettel_Web\web1\sourcecode\viettel_ns\Areas\QLVonDauTu\ReportExcelForm\KeHoachVonNam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\dungnv5\project\qlns-ctc-bqp\sourcecode\viettel_ns\Areas\QLVonDauTu\ReportExcelForm\KeHoachVonNam\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,6 +18,7 @@
   <definedNames>
     <definedName name="__dv__">#REF!</definedName>
     <definedName name="__Items__">Sheet1!$11:$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$T$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$5:$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -602,9 +603,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,11 +612,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -628,6 +626,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -644,32 +654,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -956,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,11 +975,11 @@
     <col min="10" max="10" width="21.42578125" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" customWidth="1"/>
     <col min="12" max="12" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
     <col min="14" max="14" width="26" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" customWidth="1"/>
     <col min="16" max="16" width="20.42578125" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" customWidth="1"/>
     <col min="18" max="18" width="22.28515625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="19.140625" hidden="1" customWidth="1"/>
     <col min="20" max="22" width="9.140625" hidden="1" customWidth="1"/>
@@ -1005,46 +1006,46 @@
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -1081,10 +1082,10 @@
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="40"/>
+      <c r="Q5" s="39"/>
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
       <c r="T5" s="18"/>
@@ -1093,47 +1094,47 @@
       <c r="W5" s="18"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="26" t="s">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="O6" s="29" t="s">
+      <c r="O6" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="31"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="34"/>
       <c r="R6" s="18"/>
       <c r="S6" s="18"/>
       <c r="T6" s="18"/>
@@ -1145,31 +1146,31 @@
       <c r="Z6" s="17"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="32" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="33" t="s">
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="27"/>
-      <c r="O7" s="34" t="s">
+      <c r="N7" s="26"/>
+      <c r="O7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="36" t="s">
+      <c r="P7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="37"/>
+      <c r="Q7" s="38"/>
       <c r="R7" s="18"/>
       <c r="S7" s="18"/>
       <c r="T7" s="18"/>
@@ -1181,27 +1182,27 @@
       <c r="Z7" s="17"/>
     </row>
     <row r="8" spans="1:26" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="21" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="33"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="35"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="30"/>
       <c r="P8" s="14" t="s">
         <v>10</v>
       </c>
@@ -1285,39 +1286,39 @@
       <c r="B10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="11" t="s">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="24" t="s">
+      <c r="L10" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="N10" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="O10" s="25" t="s">
+      <c r="O10" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="Q10" s="42" t="s">
         <v>75</v>
       </c>
       <c r="R10" s="18" t="s">
@@ -1364,47 +1365,47 @@
       <c r="G11" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="M11" s="20" t="s">
+      <c r="M11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="Q11" s="20" t="s">
+      <c r="Q11" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="R11" s="22" t="b">
+      <c r="R11" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="S11" s="22" t="b">
+      <c r="S11" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="T11" s="22" t="s">
+      <c r="T11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="U11" s="22"/>
-      <c r="V11" s="23">
+      <c r="U11" s="21"/>
+      <c r="V11" s="22">
         <v>2</v>
       </c>
       <c r="W11" s="18" t="s">
@@ -1417,6 +1418,9 @@
     <row r="27" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:Q7"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:Q3"/>
     <mergeCell ref="P5:Q5"/>
@@ -1433,15 +1437,15 @@
     <mergeCell ref="N6:N8"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:Q7"/>
   </mergeCells>
   <pageMargins left="0.1" right="1.1598958333333333" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="38" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"-,Italic"Trang  &amp;P</oddHeader>
   </headerFooter>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="23" max="10" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 

</xml_diff>